<commit_message>
Added a conditional in case there are no elements to display. Removed done TODO's. Updated the self-evaluation file
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -214,7 +214,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -226,12 +226,17 @@
       <name val="Helvetica"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
+      <name val="Verdana"/>
     </font>
     <font>
-      <sz val="14"/>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
@@ -357,9 +362,7 @@
       <left style="thin">
         <color indexed="8"/>
       </left>
-      <right style="thin">
-        <color indexed="9"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="8"/>
       </top>
@@ -369,12 +372,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="9"/>
-      </left>
-      <right style="thin">
-        <color indexed="9"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
         <color indexed="8"/>
       </top>
@@ -384,9 +383,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="9"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="8"/>
       </right>
@@ -409,108 +406,108 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="5" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="5" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="6" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1870,7 +1867,7 @@
         <v>14</v>
       </c>
       <c r="C9" s="20">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s" s="21">
         <v>13</v>
@@ -2409,7 +2406,7 @@
       </c>
       <c r="C51" s="35">
         <f>SUM(C6:C50)</f>
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D51" s="35">
         <v>430</v>
@@ -2428,9 +2425,6 @@
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="C7:E7"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="C7" r:id="rId1" location="" tooltip="" display=""/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>

</xml_diff>